<commit_message>
Updated excel utility and fix failing tests
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arniejumaquio/IdeaProjects/ExcelDriven/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arniejumaquio/IdeaProjects/SeleniumDataDrivenUsingExcel/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239A39D1-72A4-574B-B83B-4AA273154004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A308540-4807-A143-B8FA-28DE8DE0A0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{2A565E24-A4FE-EF4C-B9A6-F8A9B804DCD4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{2A565E24-A4FE-EF4C-B9A6-F8A9B804DCD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,38 +38,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Testcases</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>dfd</t>
-  </si>
-  <si>
-    <t>hasdha</t>
-  </si>
-  <si>
-    <t>sdadsas</t>
-  </si>
-  <si>
     <t>Purchase</t>
   </si>
   <si>
-    <t>erewqe</t>
-  </si>
-  <si>
     <t>Add Profile</t>
   </si>
   <si>
@@ -79,9 +58,6 @@
     <t>asjdasd</t>
   </si>
   <si>
-    <t>sdas</t>
-  </si>
-  <si>
     <t>Delete Profile</t>
   </si>
   <si>
@@ -91,10 +67,19 @@
     <t>bdasnd</t>
   </si>
   <si>
-    <t>tqwet</t>
-  </si>
-  <si>
     <t>rahulshettyacademy@mailiantor.com</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>unknownuuid8123712@mailinator.com</t>
+  </si>
+  <si>
+    <t>Test1234@!</t>
   </si>
 </sst>
 </file>
@@ -477,87 +462,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81596029-05C8-0C46-A9E4-AE51481628C4}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>123456</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{1805777E-3EF8-AF4E-88E1-E8EAC4433551}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{CF0E09AA-B0AF-1E4A-B12D-0931618C4BC5}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{B1284A2B-717B-0E4A-BFE1-F0F83FAEF323}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>